<commit_message>
[IX-1] Updated Add,Search,Update Functionalities
</commit_message>
<xml_diff>
--- a/backend/excel/batchmates.xlsx
+++ b/backend/excel/batchmates.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -508,9 +508,674 @@
         <v/>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="B3" t="str">
+        <v>JavaScript</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Node.js, Express, MongoDB</v>
+      </c>
+      <c r="D3" t="str">
+        <v>6</v>
+      </c>
+      <c r="E3" t="str">
+        <v>7 years</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Senior Developer</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Retail, Finance</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Selenium, JUnit, TestNG, Cypress</v>
+      </c>
+      <c r="I3" t="str">
+        <v>Docker, Jenkins, Git, Kubernetes</v>
+      </c>
+      <c r="J3" t="str">
+        <v>AWS, Azure</v>
+      </c>
+      <c r="K3" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="L3" t="str">
+        <v>Teamcenter customization</v>
+      </c>
+      <c r="M3" t="str">
+        <v>System Testing</v>
+      </c>
+      <c r="N3" t="str">
+        <v>Issue resolution</v>
+      </c>
+      <c r="O3" t="str">
+        <v>Server config</v>
+      </c>
+      <c r="P3" t="str">
+        <v>TC 11 to TC 13</v>
+      </c>
+      <c r="Q3" t="str">
+        <v>NX integration</v>
+      </c>
+      <c r="R3" t="str">
+        <v>SOA services</v>
+      </c>
+      <c r="S3" t="str">
+        <v>SAP connector</v>
+      </c>
+      <c r="T3" t="str">
+        <v>Technomatix</v>
+      </c>
+      <c r="U3" t="str">
+        <v>Quality check flows</v>
+      </c>
+      <c r="V3" t="str">
+        <v>OOP, design patterns</v>
+      </c>
+      <c r="W3" t="str">
+        <v>Handled 6 members</v>
+      </c>
+      <c r="X3" t="str">
+        <v>BOM management</v>
+      </c>
+      <c r="Y3" t="str">
+        <v>Data migration from Windchill</v>
+      </c>
+      <c r="Z3" t="str">
+        <v>Variant rules setup</v>
+      </c>
+      <c r="AA3" t="str">
+        <v>Custom widgets</v>
+      </c>
+      <c r="AB3" t="str">
+        <v>Change Management, Structure Manager</v>
+      </c>
+      <c r="AC3" t="str">
+        <v>AWS Certified Developer</v>
+      </c>
+      <c r="AD3" t="str">
+        <v>Google Cloud Associate</v>
+      </c>
+      <c r="AE3" t="str">
+        <v>Available for mentoring</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>John Doel</v>
+      </c>
+      <c r="B4" t="str">
+        <v>JavaScript</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Node.js, Express, MongoDB</v>
+      </c>
+      <c r="D4" t="str">
+        <v>6</v>
+      </c>
+      <c r="E4" t="str">
+        <v>7 years</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Senior Developer</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Retail, Finance</v>
+      </c>
+      <c r="H4" t="str">
+        <v>Selenium, JUnit, TestNG, Cypress</v>
+      </c>
+      <c r="I4" t="str">
+        <v>Docker, Jenkins, Git, Kubernetes</v>
+      </c>
+      <c r="J4" t="str">
+        <v>AWS, Azure</v>
+      </c>
+      <c r="K4" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="L4" t="str">
+        <v>Teamcenter customization</v>
+      </c>
+      <c r="M4" t="str">
+        <v>System Testing</v>
+      </c>
+      <c r="N4" t="str">
+        <v>Issue resolution</v>
+      </c>
+      <c r="O4" t="str">
+        <v>Server config</v>
+      </c>
+      <c r="P4" t="str">
+        <v>TC 11 to TC 13</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>NX integration</v>
+      </c>
+      <c r="R4" t="str">
+        <v>SOA services</v>
+      </c>
+      <c r="S4" t="str">
+        <v>SAP connector</v>
+      </c>
+      <c r="T4" t="str">
+        <v>Technomatix</v>
+      </c>
+      <c r="U4" t="str">
+        <v>Quality check flows</v>
+      </c>
+      <c r="V4" t="str">
+        <v>OOP, design patterns</v>
+      </c>
+      <c r="W4" t="str">
+        <v>Handled 6 members</v>
+      </c>
+      <c r="X4" t="str">
+        <v>BOM management</v>
+      </c>
+      <c r="Y4" t="str">
+        <v>Data migration from Windchill</v>
+      </c>
+      <c r="Z4" t="str">
+        <v>Variant rules setup</v>
+      </c>
+      <c r="AA4" t="str">
+        <v>Custom widgets</v>
+      </c>
+      <c r="AB4" t="str">
+        <v>Change Management, Structure Manager</v>
+      </c>
+      <c r="AC4" t="str">
+        <v>AWS Certified Developer</v>
+      </c>
+      <c r="AD4" t="str">
+        <v>Google Cloud Associate</v>
+      </c>
+      <c r="AE4" t="str">
+        <v>Available for mentoring</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>John Doel</v>
+      </c>
+      <c r="B5" t="str">
+        <v>JavaScript</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Node.js, Express, MongoDB</v>
+      </c>
+      <c r="D5" t="str">
+        <v>6</v>
+      </c>
+      <c r="E5" t="str">
+        <v>7 years</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Senior Developer</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Retail, Finance</v>
+      </c>
+      <c r="H5" t="str">
+        <v>Selenium, JUnit, TestNG, Cypress</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Docker, Jenkins, Git, Kubernetes</v>
+      </c>
+      <c r="J5" t="str">
+        <v>AWS, Azure</v>
+      </c>
+      <c r="K5" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="L5" t="str">
+        <v>Teamcenter customization</v>
+      </c>
+      <c r="M5" t="str">
+        <v>System Testing</v>
+      </c>
+      <c r="N5" t="str">
+        <v>Issue resolution</v>
+      </c>
+      <c r="O5" t="str">
+        <v>Server config</v>
+      </c>
+      <c r="P5" t="str">
+        <v>TC 11 to TC 13</v>
+      </c>
+      <c r="Q5" t="str">
+        <v>NX integration</v>
+      </c>
+      <c r="R5" t="str">
+        <v>SOA services</v>
+      </c>
+      <c r="S5" t="str">
+        <v>SAP connector</v>
+      </c>
+      <c r="T5" t="str">
+        <v>Technomatix</v>
+      </c>
+      <c r="U5" t="str">
+        <v>Quality check flows</v>
+      </c>
+      <c r="V5" t="str">
+        <v>OOP, design patterns</v>
+      </c>
+      <c r="W5" t="str">
+        <v>Handled 6 members</v>
+      </c>
+      <c r="X5" t="str">
+        <v>BOM management</v>
+      </c>
+      <c r="Y5" t="str">
+        <v>Data migration from Windchill</v>
+      </c>
+      <c r="Z5" t="str">
+        <v>Variant rules setup</v>
+      </c>
+      <c r="AA5" t="str">
+        <v>Custom widgets</v>
+      </c>
+      <c r="AB5" t="str">
+        <v>Change Management, Structure Manager</v>
+      </c>
+      <c r="AC5" t="str">
+        <v>AWS Certified Developer</v>
+      </c>
+      <c r="AD5" t="str">
+        <v>Google Cloud Associate</v>
+      </c>
+      <c r="AE5" t="str">
+        <v>Available for mentoring</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>John Doel</v>
+      </c>
+      <c r="B6" t="str">
+        <v>JavaScript</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Node.js, Express, MongoDB</v>
+      </c>
+      <c r="D6" t="str">
+        <v>6</v>
+      </c>
+      <c r="E6" t="str">
+        <v>7 years</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Senior Developer</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Retail, Finance</v>
+      </c>
+      <c r="H6" t="str">
+        <v>Selenium, JUnit, TestNG, Cypress</v>
+      </c>
+      <c r="I6" t="str">
+        <v>Docker, Jenkins, Git, Kubernetes</v>
+      </c>
+      <c r="J6" t="str">
+        <v>AWS, Azure</v>
+      </c>
+      <c r="K6" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="L6" t="str">
+        <v>Teamcenter customization</v>
+      </c>
+      <c r="M6" t="str">
+        <v>System Testing</v>
+      </c>
+      <c r="N6" t="str">
+        <v>Issue resolution</v>
+      </c>
+      <c r="O6" t="str">
+        <v>Server config</v>
+      </c>
+      <c r="P6" t="str">
+        <v>TC 11 to TC 13</v>
+      </c>
+      <c r="Q6" t="str">
+        <v>NX integration</v>
+      </c>
+      <c r="R6" t="str">
+        <v>SOA services</v>
+      </c>
+      <c r="S6" t="str">
+        <v>SAP connector</v>
+      </c>
+      <c r="T6" t="str">
+        <v>Technomatix</v>
+      </c>
+      <c r="U6" t="str">
+        <v>Quality check flows</v>
+      </c>
+      <c r="V6" t="str">
+        <v>OOP, design patterns</v>
+      </c>
+      <c r="W6" t="str">
+        <v>Handled 6 members</v>
+      </c>
+      <c r="X6" t="str">
+        <v>BOM management</v>
+      </c>
+      <c r="Y6" t="str">
+        <v>Data migration from Windchill</v>
+      </c>
+      <c r="Z6" t="str">
+        <v>Variant rules setup</v>
+      </c>
+      <c r="AA6" t="str">
+        <v>Custom widgets</v>
+      </c>
+      <c r="AB6" t="str">
+        <v>Change Management, Structure Manager</v>
+      </c>
+      <c r="AC6" t="str">
+        <v>AWS Certified Developer</v>
+      </c>
+      <c r="AD6" t="str">
+        <v>Google Cloud Associate</v>
+      </c>
+      <c r="AE6" t="str">
+        <v>Available for mentoring</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>John Doel</v>
+      </c>
+      <c r="B7" t="str">
+        <v>JavaScript</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Node.js, Express, MongoDB</v>
+      </c>
+      <c r="D7" t="str">
+        <v>6</v>
+      </c>
+      <c r="E7" t="str">
+        <v>7 years</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Senior Developer</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Retail, Finance</v>
+      </c>
+      <c r="H7" t="str">
+        <v>Selenium, JUnit, TestNG, Cypress</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Docker, Jenkins, Git, Kubernetes</v>
+      </c>
+      <c r="J7" t="str">
+        <v>AWS, Azure</v>
+      </c>
+      <c r="K7" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="L7" t="str">
+        <v>Teamcenter customization</v>
+      </c>
+      <c r="M7" t="str">
+        <v>System Testing</v>
+      </c>
+      <c r="N7" t="str">
+        <v>Issue resolution</v>
+      </c>
+      <c r="O7" t="str">
+        <v>Server config</v>
+      </c>
+      <c r="P7" t="str">
+        <v>TC 11 to TC 13</v>
+      </c>
+      <c r="Q7" t="str">
+        <v>NX integration</v>
+      </c>
+      <c r="R7" t="str">
+        <v>SOA services</v>
+      </c>
+      <c r="S7" t="str">
+        <v>SAP connector</v>
+      </c>
+      <c r="T7" t="str">
+        <v>Technomatix</v>
+      </c>
+      <c r="U7" t="str">
+        <v>Quality check flows</v>
+      </c>
+      <c r="V7" t="str">
+        <v>OOP, design patterns</v>
+      </c>
+      <c r="W7" t="str">
+        <v>Handled 6 members</v>
+      </c>
+      <c r="X7" t="str">
+        <v>BOM management</v>
+      </c>
+      <c r="Y7" t="str">
+        <v>Data migration from Windchill</v>
+      </c>
+      <c r="Z7" t="str">
+        <v>Variant rules setup</v>
+      </c>
+      <c r="AA7" t="str">
+        <v>Custom widgets</v>
+      </c>
+      <c r="AB7" t="str">
+        <v>Change Management, Structure Manager</v>
+      </c>
+      <c r="AC7" t="str">
+        <v>AWS Certified Developer</v>
+      </c>
+      <c r="AD7" t="str">
+        <v>Google Cloud Associate</v>
+      </c>
+      <c r="AE7" t="str">
+        <v>Available for mentoring</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>John Doel</v>
+      </c>
+      <c r="B8" t="str">
+        <v>JavaScript</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Node.js, Express, MongoDB</v>
+      </c>
+      <c r="D8" t="str">
+        <v>6</v>
+      </c>
+      <c r="E8" t="str">
+        <v>7 years</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Senior Developer</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Retail, Finance</v>
+      </c>
+      <c r="H8" t="str">
+        <v>Selenium, JUnit, TestNG, Cypress</v>
+      </c>
+      <c r="I8" t="str">
+        <v>Docker, Jenkins, Git, Kubernetes</v>
+      </c>
+      <c r="J8" t="str">
+        <v>AWS, Azure</v>
+      </c>
+      <c r="K8" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="L8" t="str">
+        <v>Teamcenter customization</v>
+      </c>
+      <c r="M8" t="str">
+        <v>System Testing</v>
+      </c>
+      <c r="N8" t="str">
+        <v>Issue resolution</v>
+      </c>
+      <c r="O8" t="str">
+        <v>Server config</v>
+      </c>
+      <c r="P8" t="str">
+        <v>TC 11 to TC 13</v>
+      </c>
+      <c r="Q8" t="str">
+        <v>NX integration</v>
+      </c>
+      <c r="R8" t="str">
+        <v>SOA services</v>
+      </c>
+      <c r="S8" t="str">
+        <v>SAP connector</v>
+      </c>
+      <c r="T8" t="str">
+        <v>Technomatix</v>
+      </c>
+      <c r="U8" t="str">
+        <v>Quality check flows</v>
+      </c>
+      <c r="V8" t="str">
+        <v>OOP, design patterns</v>
+      </c>
+      <c r="W8" t="str">
+        <v>Handled 6 members</v>
+      </c>
+      <c r="X8" t="str">
+        <v>BOM management</v>
+      </c>
+      <c r="Y8" t="str">
+        <v>Data migration from Windchill</v>
+      </c>
+      <c r="Z8" t="str">
+        <v>Variant rules setup</v>
+      </c>
+      <c r="AA8" t="str">
+        <v>Custom widgets</v>
+      </c>
+      <c r="AB8" t="str">
+        <v>Change Management, Structure Manager</v>
+      </c>
+      <c r="AC8" t="str">
+        <v>AWS Certified Developer</v>
+      </c>
+      <c r="AD8" t="str">
+        <v>Google Cloud Associate</v>
+      </c>
+      <c r="AE8" t="str">
+        <v>Available for mentoring</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>John Doel</v>
+      </c>
+      <c r="B9" t="str">
+        <v>JavaScript</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Node.js, Express, MongoDB</v>
+      </c>
+      <c r="D9" t="str">
+        <v>6</v>
+      </c>
+      <c r="E9" t="str">
+        <v>7 years</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Senior Developer</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Retail, Finance</v>
+      </c>
+      <c r="H9" t="str">
+        <v>Selenium, JUnit, TestNG, Cypress</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Docker, Jenkins, Git, Kubernetes</v>
+      </c>
+      <c r="J9" t="str">
+        <v>AWS, Azure</v>
+      </c>
+      <c r="K9" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="L9" t="str">
+        <v>Teamcenter customization</v>
+      </c>
+      <c r="M9" t="str">
+        <v>System Testing</v>
+      </c>
+      <c r="N9" t="str">
+        <v>Issue resolution</v>
+      </c>
+      <c r="O9" t="str">
+        <v>Server config</v>
+      </c>
+      <c r="P9" t="str">
+        <v>TC 11 to TC 13</v>
+      </c>
+      <c r="Q9" t="str">
+        <v>NX integration</v>
+      </c>
+      <c r="R9" t="str">
+        <v>SOA services</v>
+      </c>
+      <c r="S9" t="str">
+        <v>SAP connector</v>
+      </c>
+      <c r="T9" t="str">
+        <v>Technomatix</v>
+      </c>
+      <c r="U9" t="str">
+        <v>Quality check flows</v>
+      </c>
+      <c r="V9" t="str">
+        <v>OOP, design patterns</v>
+      </c>
+      <c r="W9" t="str">
+        <v>Handled 6 members</v>
+      </c>
+      <c r="X9" t="str">
+        <v>BOM management</v>
+      </c>
+      <c r="Y9" t="str">
+        <v>Data migration from Windchill</v>
+      </c>
+      <c r="Z9" t="str">
+        <v>Variant rules setup</v>
+      </c>
+      <c r="AA9" t="str">
+        <v>Custom widgets</v>
+      </c>
+      <c r="AB9" t="str">
+        <v>Change Management, Structure Manager</v>
+      </c>
+      <c r="AC9" t="str">
+        <v>AWS Certified Developer</v>
+      </c>
+      <c r="AD9" t="str">
+        <v>Google Cloud Associate</v>
+      </c>
+      <c r="AE9" t="str">
+        <v>Available for mentoring</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IX-8: Updated Home, Profile, Search, Add, Model and Controller
</commit_message>
<xml_diff>
--- a/backend/excel/batchmates.xlsx
+++ b/backend/excel/batchmates.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE10"/>
+  <dimension ref="A1:AE13"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1268,9 +1268,33 @@
         <v>PLM SME with 2 migrations handled</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Sowbi</v>
+      </c>
+      <c r="AC11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Hari</v>
+      </c>
+      <c r="AC12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Hari</v>
+      </c>
+      <c r="AC13" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IX-11: Updated batchmatecontroller/routes files
</commit_message>
<xml_diff>
--- a/backend/excel/batchmates.xlsx
+++ b/backend/excel/batchmates.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE13"/>
+  <dimension ref="A1:AE18"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1292,9 +1292,49 @@
         <v/>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Hari</v>
+      </c>
+      <c r="AC14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Hari</v>
+      </c>
+      <c r="AC15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>hari</v>
+      </c>
+      <c r="AC16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>ADITYA</v>
+      </c>
+      <c r="AC17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Harithaa</v>
+      </c>
+      <c r="AC18" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Batchmate model,login controller,routes,server.js,installed packages for mail service
</commit_message>
<xml_diff>
--- a/backend/excel/batchmates.xlsx
+++ b/backend/excel/batchmates.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE18"/>
+  <dimension ref="A1:AE20"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1332,9 +1332,25 @@
         <v/>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Jane Doe</v>
+      </c>
+      <c r="AC19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Sowbaranika.G</v>
+      </c>
+      <c r="AC20" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE20"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IX-22: Updated currentrole, worklocation's controller and routes
</commit_message>
<xml_diff>
--- a/backend/excel/batchmates.xlsx
+++ b/backend/excel/batchmates.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE18"/>
+  <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1332,9 +1332,17 @@
         <v/>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Manoj</v>
+      </c>
+      <c r="AC19" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE19"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IX-28: Updated Login Functionality
</commit_message>
<xml_diff>
--- a/backend/excel/batchmates.xlsx
+++ b/backend/excel/batchmates.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE19"/>
+  <dimension ref="A1:AE22"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1340,9 +1340,33 @@
         <v/>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Harish K</v>
+      </c>
+      <c r="AC20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Srujan Kumar</v>
+      </c>
+      <c r="AC21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Sowbaranika</v>
+      </c>
+      <c r="AC22" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE22"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IX-31: Switched to a central database,updated some controller codes
</commit_message>
<xml_diff>
--- a/backend/excel/batchmates.xlsx
+++ b/backend/excel/batchmates.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE22"/>
+  <dimension ref="A1:AE23"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1364,9 +1364,17 @@
         <v/>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Minnal Harish</v>
+      </c>
+      <c r="AC23" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE22"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE23"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IX-34: Added admin and user access restriction
</commit_message>
<xml_diff>
--- a/backend/excel/batchmates.xlsx
+++ b/backend/excel/batchmates.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE23"/>
+  <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1372,9 +1372,17 @@
         <v/>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Harish Kotakonda Govindarajulu</v>
+      </c>
+      <c r="AC24" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE23"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE24"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update PLM Cad Integrations Controller
</commit_message>
<xml_diff>
--- a/backend/excel/batchmates.xlsx
+++ b/backend/excel/batchmates.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE24"/>
+  <dimension ref="A1:AE25"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1380,9 +1380,17 @@
         <v/>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Minnal Harish</v>
+      </c>
+      <c r="AC25" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE24"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE25"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>